<commit_message>
JS 8 - Praktikum 3
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester_4\PemrogramanWeb\laragon\www\PWL_POS\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{155DD728-9793-4021-A9B3-4BFDB88C88B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C587D2-3ED4-4A0C-9D54-73D801E73A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{0D4CA07C-D14C-4C68-B4FC-7AAF55D8D7BE}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="10545" windowHeight="10875" xr2:uid="{0D4CA07C-D14C-4C68-B4FC-7AAF55D8D7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,16 +445,16 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -505,7 +505,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -522,7 +522,7 @@
         <v>18500</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -539,7 +539,7 @@
         <v>92500</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>